<commit_message>
Update Simple Linear Regression.xlsx
</commit_message>
<xml_diff>
--- a/Simple Linear Regression.xlsx
+++ b/Simple Linear Regression.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Teaching\L6 Data Science\L6 DS Final Documents\M5 Data Science Professional Practice\GitHub\demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Teaching\L6 Data Science\L6 DS Final Documents\M5 Data Science Professional Practice\GitHub\portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{709F1757-9AEA-4869-AF6A-6F7E0B3AD772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E404AC-A1A3-412C-B4E5-15AFB91F5C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4215" yWindow="2520" windowWidth="17460" windowHeight="12960" activeTab="1" xr2:uid="{62682CF4-A5DE-4CA0-BAA7-BD66514D1DB8}"/>
   </bookViews>
@@ -3008,7 +3008,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3045,7 +3045,7 @@
         <v>29</v>
       </c>
       <c r="F2" s="2">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>